<commit_message>
need to put comments on the result.
</commit_message>
<xml_diff>
--- a/HW2/result.xlsx
+++ b/HW2/result.xlsx
@@ -2751,7 +2751,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3343,11 +3343,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="42589878"/>
-        <c:axId val="79806607"/>
+        <c:axId val="32916302"/>
+        <c:axId val="78616212"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42589878"/>
+        <c:axId val="32916302"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3384,14 +3384,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79806607"/>
+        <c:crossAx val="78616212"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79806607"/>
+        <c:axId val="78616212"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3428,7 +3428,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42589878"/>
+        <c:crossAx val="32916302"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3476,7 +3476,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3573,11 +3573,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="19334195"/>
-        <c:axId val="63414110"/>
+        <c:axId val="95852748"/>
+        <c:axId val="27477517"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="19334195"/>
+        <c:axId val="95852748"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3605,14 +3605,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63414110"/>
+        <c:crossAx val="27477517"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63414110"/>
+        <c:axId val="27477517"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3649,7 +3649,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19334195"/>
+        <c:crossAx val="95852748"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3707,10 +3707,10 @@
       <xdr:rowOff>20880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>147600</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>8640</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>51480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3719,7 +3719,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1673640" y="1393560"/>
-        <a:ext cx="7328520" cy="3865680"/>
+        <a:ext cx="5605560" cy="2956680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3731,16 +3731,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>36360</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>23040</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>14040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>106560</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>93240</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3748,7 +3748,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8932680" y="686160"/>
+        <a:off x="1604160" y="4475520"/>
         <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
@@ -3770,7 +3770,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>